<commit_message>
fix requisites tables - xlsx
</commit_message>
<xml_diff>
--- a/analysis/requisitesTable.xlsx
+++ b/analysis/requisitesTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giuliobosco/drive/aa_SAMT1819/progetti/progetto1/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470C122B-41A0-C141-8A1C-1E80B53B89EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C6E6F5-1761-9C4B-9FCC-D941565B156A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22400" xr2:uid="{1D4C3A32-79B6-014E-9230-2ADD48425820}"/>
   </bookViews>
@@ -141,9 +141,6 @@
     <t>tasto -&gt; controllo</t>
   </si>
   <si>
-    <t>tasto -&gt; iscrizione</t>
-  </si>
-  <si>
     <t>ritorno a pagina benvenuto</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>Salvare i file in 2 CSV (Registrazioni_tutte.csv, Registrazione_yyyy_mm_dd.csv)</t>
+  </si>
+  <si>
+    <t>tasto -&gt; iscrizione, salvare i dati e andare alla pagina lettura dati</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -595,7 +595,7 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G3" t="s">
         <v>22</v>
@@ -604,7 +604,7 @@
         <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -705,7 +705,7 @@
         <v>36</v>
       </c>
       <c r="H7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -731,7 +731,7 @@
         <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>